<commit_message>
fix bt upload duty bug
</commit_message>
<xml_diff>
--- a/bt_mesh_sig_cold_warm/DOC/flash分配.xlsx
+++ b/bt_mesh_sig_cold_warm/DOC/flash分配.xlsx
@@ -8,15 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>全局变量</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -70,91 +68,158 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>lightvalue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XRBoffbrightvalue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x2F05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lowlightDELAY_NUM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x2F06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SWITCHfXBR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x2F07</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resetbtcnt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x2F80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>光照门限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雷达开关</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关灯延时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓝牙重新连接次数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感应延时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雷达感应门限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不开雷达时的亮度值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>temper_value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冷暖度值0~100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>灯亮度值0~100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linkage_flag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>联动开关</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x2F08</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SWITCHflag2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开关灯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x2F09</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>all_day_micro_light_enable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全天伴亮开关</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x2F0A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x2F0B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bt_and_sigmesh_duty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓝牙及mesh通信周期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>0x2F03~0x2F04</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>lightvalue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>XRBoffbrightvalue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x2F05</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lowlightDELAY_NUM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x2F06</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SWITCHfXBR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x2F07</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>resetbtcnt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x2F80</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>光照门限</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>雷达开关</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>关灯延时</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>蓝牙重新连接次数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>感应延时</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>雷达感应门限</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>不开雷达时的亮度值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>temper_value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>u8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>冷暖度值0~100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>灯亮度值0~100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x2F08</t>
+    <t>0x2F0C~0x2F0D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x2F81</t>
+  </si>
+  <si>
+    <t>bt_join_cnt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓝牙配网标志</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -557,16 +622,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11.73046875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.19921875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.265625" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.9296875" style="2" customWidth="1"/>
     <col min="4" max="4" width="21.73046875" style="2" customWidth="1"/>
     <col min="5" max="5" width="21" style="2" customWidth="1"/>
@@ -601,7 +666,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
@@ -621,7 +686,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>11</v>
@@ -638,10 +703,10 @@
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -649,16 +714,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -666,13 +731,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="4"/>
     </row>
@@ -681,16 +746,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -698,16 +763,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -715,16 +780,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -732,19 +797,104 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="2">
+      <c r="F14" s="2">
         <v>12160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -755,32 +905,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>